<commit_message>
Added automatic cell height calculation
</commit_message>
<xml_diff>
--- a/sample/template.xlsx
+++ b/sample/template.xlsx
@@ -356,7 +356,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -471,7 +471,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>